<commit_message>
Added data logging, and heading and height to path/tuple
</commit_message>
<xml_diff>
--- a/PacketIndex.xlsx
+++ b/PacketIndex.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Dropbox\School-Ben\University\Third Year (2017-2018)\Aero\GroundStationGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB271CDE-AEFF-461F-8DEE-6B042340B562}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="7833" xr2:uid="{86DC4640-F2E8-423C-B24A-DAE3C2ECEA38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Data</t>
   </si>
@@ -72,6 +73,9 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>heading</t>
   </si>
 </sst>
 </file>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953CF21C-7A7E-4B0F-AF11-078ED090BA89}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -473,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D14" si="0">C3-B3</f>
         <v>2</v>
       </c>
     </row>
@@ -591,50 +595,66 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f>SUM(B$2:B11)</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D11" si="1">C11-B11</f>
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
         <f>SUM(B$2:B12)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>SUM(B$2:B13)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <f>SUM(B$2:B14)</f>
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up code and commentted + fixed picture packet parsing
</commit_message>
<xml_diff>
--- a/PacketIndex.xlsx
+++ b/PacketIndex.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Dropbox\School-Ben\University\Third Year (2017-2018)\Aero\GroundStationGUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ground-Station-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB271CDE-AEFF-461F-8DEE-6B042340B562}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595A831-B1D0-4D28-9CEC-441C326A0935}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="7833" xr2:uid="{86DC4640-F2E8-423C-B24A-DAE3C2ECEA38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="7833" activeTab="1" xr2:uid="{86DC4640-F2E8-423C-B24A-DAE3C2ECEA38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data packet" sheetId="1" r:id="rId1"/>
+    <sheet name="Point packet" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Data</t>
   </si>
@@ -429,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953CF21C-7A7E-4B0F-AF11-078ED090BA89}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -660,4 +661,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9954FF-56C9-4385-94B5-CD42DD62A611}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>SUM(B$2:B2)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>SUM(B$2:B3)</f>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">C3-B3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>SUM(B$2:B4)</f>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>SUM(B$2:B5)</f>
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f>SUM(B$2:B6)</f>
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f>SUM(B$2:B7)</f>
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f>SUM(B$2:B8)</f>
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>